<commit_message>
fixed reading time and loop
</commit_message>
<xml_diff>
--- a/csc-501-project-1/measurements.xlsx
+++ b/csc-501-project-1/measurements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Loops" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,6 @@
   </si>
   <si>
     <t>Without read time</t>
-  </si>
-  <si>
-    <t>with read (100000 chars) cycles</t>
-  </si>
-  <si>
-    <t>With read (100000 chars) time</t>
   </si>
   <si>
     <t>Without procedure cycles</t>
@@ -209,6 +203,12 @@
   </si>
   <si>
     <t>Time (microseconds)</t>
+  </si>
+  <si>
+    <t>with read cycles</t>
+  </si>
+  <si>
+    <t>With read time</t>
   </si>
 </sst>
 </file>
@@ -464,49 +464,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>38840.33</c:v>
+                  <c:v>40316.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>164886.87</c:v>
+                  <c:v>34745.43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>196.53</c:v>
+                  <c:v>13.07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>197.52</c:v>
+                  <c:v>14.06</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>244.44</c:v>
+                  <c:v>427.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>227.5</c:v>
+                  <c:v>44.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>214.1</c:v>
+                  <c:v>30.63999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>234.51</c:v>
+                  <c:v>51.04999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>250.5</c:v>
+                  <c:v>67.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>221.95</c:v>
+                  <c:v>405.41</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4847.25</c:v>
+                  <c:v>4682.63</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>486234.8</c:v>
+                  <c:v>486080.99</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.86398792E6</c:v>
+                  <c:v>750607.3599999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35167.36</c:v>
+                  <c:v>35012.16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>39940.1</c:v>
+                  <c:v>39771.93</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>243256.68</c:v>
@@ -525,11 +525,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="42125296"/>
-        <c:axId val="43564416"/>
+        <c:axId val="168882800"/>
+        <c:axId val="168886080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42125296"/>
+        <c:axId val="168882800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -571,7 +571,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43564416"/>
+        <c:crossAx val="168886080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -579,7 +579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43564416"/>
+        <c:axId val="168886080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,7 +628,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42125296"/>
+        <c:crossAx val="168882800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -862,49 +862,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>23.88</c:v>
+                  <c:v>25.84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.01</c:v>
+                  <c:v>21.65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15</c:v>
+                  <c:v>0.07</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15</c:v>
+                  <c:v>0.07</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.16</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.1</c:v>
+                  <c:v>2.06</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>153.46</c:v>
+                  <c:v>153.41</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1314.86</c:v>
+                  <c:v>522.4099999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.39</c:v>
+                  <c:v>21.34</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25.58</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>161.83</c:v>
@@ -923,11 +923,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="42110832"/>
-        <c:axId val="42832544"/>
+        <c:axId val="168900704"/>
+        <c:axId val="168903456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42110832"/>
+        <c:axId val="168900704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42832544"/>
+        <c:crossAx val="168903456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -977,7 +977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42832544"/>
+        <c:axId val="168903456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1026,7 +1026,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42110832"/>
+        <c:crossAx val="168900704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2163,13 +2163,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>10160</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:colOff>802640</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
     </xdr:to>
@@ -2193,13 +2193,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>10160</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>193040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>193040</xdr:rowOff>
     </xdr:to>
@@ -2489,8 +2489,8 @@
   <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="118" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2517,52 +2517,52 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B2">
-        <v>51081</v>
+        <v>51184</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B3">
-        <v>37866</v>
+        <v>37796</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B4">
-        <v>37864</v>
+        <v>37954</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B5">
-        <v>37846</v>
+        <v>37952</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2573,16 +2573,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B6">
-        <v>37854</v>
+        <v>37920</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2590,27 +2590,27 @@
         <v>144</v>
       </c>
       <c r="B7">
-        <v>37894</v>
+        <v>37918</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B8">
-        <v>37936</v>
+        <v>37948</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2618,49 +2618,49 @@
         <v>144</v>
       </c>
       <c r="B9">
-        <v>37894</v>
+        <v>40876</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B10">
-        <v>37908</v>
+        <v>37812</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="B11">
-        <v>37864</v>
+        <v>37908</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B12">
-        <v>37814</v>
+        <v>40954</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2674,13 +2674,13 @@
         <v>144</v>
       </c>
       <c r="B13">
-        <v>37858</v>
+        <v>37836</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2688,7 +2688,7 @@
         <v>154</v>
       </c>
       <c r="B14">
-        <v>37156</v>
+        <v>37948</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2699,10 +2699,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B15">
-        <v>37946</v>
+        <v>40862</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2713,38 +2713,38 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>207</v>
+        <v>146</v>
       </c>
       <c r="B16">
-        <v>37870</v>
+        <v>37992</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B17">
-        <v>37810</v>
+        <v>37862</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B18">
-        <v>37834</v>
+        <v>40948</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2755,10 +2755,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B19">
-        <v>37936</v>
+        <v>37928</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2769,10 +2769,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B20">
-        <v>37882</v>
+        <v>37848</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2783,80 +2783,80 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B21">
-        <v>37898</v>
+        <v>37910</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B22">
-        <v>37936</v>
+        <v>37910</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B23">
-        <v>37824</v>
+        <v>40850</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B24">
-        <v>37786</v>
+        <v>37822</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B25">
-        <v>37862</v>
+        <v>37858</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B26">
-        <v>37864</v>
+        <v>37854</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -2867,10 +2867,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="B27">
-        <v>37906</v>
+        <v>37784</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2881,52 +2881,52 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B28">
-        <v>37890</v>
+        <v>37920</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="B29">
-        <v>38654</v>
+        <v>40950</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="B30">
-        <v>37840</v>
+        <v>37850</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B31">
-        <v>37988</v>
+        <v>37858</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2937,38 +2937,38 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B32">
-        <v>37906</v>
+        <v>37910</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B33">
-        <v>37868</v>
+        <v>37858</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B34">
-        <v>37906</v>
+        <v>37988</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2979,80 +2979,80 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B35">
-        <v>37846</v>
+        <v>37854</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B36">
-        <v>37714</v>
+        <v>37822</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B37">
-        <v>37908</v>
+        <v>37928</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B38">
-        <v>37912</v>
+        <v>37822</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B39">
-        <v>37916</v>
+        <v>37822</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B40">
-        <v>37926</v>
+        <v>37820</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -3063,10 +3063,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B41">
-        <v>37904</v>
+        <v>37822</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -3077,30 +3077,30 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B42">
-        <v>37946</v>
+        <v>37956</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B43">
-        <v>51582</v>
+        <v>37946</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -3108,7 +3108,7 @@
         <v>154</v>
       </c>
       <c r="B44">
-        <v>37840</v>
+        <v>37922</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -3119,24 +3119,24 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B45">
-        <v>37906</v>
+        <v>40950</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B46">
-        <v>37896</v>
+        <v>37830</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -3147,38 +3147,38 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B47">
-        <v>37788</v>
+        <v>37956</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B48">
-        <v>37856</v>
+        <v>37822</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B49">
-        <v>37846</v>
+        <v>37858</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -3189,38 +3189,38 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="B50">
-        <v>37644</v>
+        <v>40948</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B51">
-        <v>37866</v>
+        <v>37846</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
       <c r="D51">
-        <v>24</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B52">
-        <v>37900</v>
+        <v>37848</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -3231,24 +3231,24 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B53">
-        <v>37820</v>
+        <v>37858</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B54">
-        <v>37830</v>
+        <v>37852</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -3259,13 +3259,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B55">
-        <v>37880</v>
+        <v>37948</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>23</v>
@@ -3273,10 +3273,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B56">
-        <v>37870</v>
+        <v>37850</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -3287,24 +3287,24 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B57">
-        <v>37470</v>
+        <v>37864</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B58">
-        <v>37780</v>
+        <v>37784</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -3315,10 +3315,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B59">
-        <v>37834</v>
+        <v>40950</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -3329,13 +3329,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B60">
-        <v>37920</v>
+        <v>54598</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60">
         <v>23</v>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B61">
         <v>37864</v>
@@ -3352,43 +3352,43 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B62">
-        <v>37852</v>
+        <v>37854</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B63">
-        <v>37924</v>
+        <v>37952</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B64">
-        <v>37926</v>
+        <v>40890</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -3399,24 +3399,24 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B65">
-        <v>37906</v>
+        <v>37850</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B66">
-        <v>37864</v>
+        <v>37812</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -3430,7 +3430,7 @@
         <v>144</v>
       </c>
       <c r="B67">
-        <v>37860</v>
+        <v>37998</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -3441,10 +3441,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B68">
-        <v>37816</v>
+        <v>40942</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -3455,16 +3455,16 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B69">
-        <v>37866</v>
+        <v>37858</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -3472,13 +3472,13 @@
         <v>144</v>
       </c>
       <c r="B70">
-        <v>37814</v>
+        <v>41000</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -3486,7 +3486,7 @@
         <v>144</v>
       </c>
       <c r="B71">
-        <v>37844</v>
+        <v>37862</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -3497,80 +3497,80 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B72">
-        <v>37900</v>
+        <v>163434</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B73">
-        <v>37854</v>
+        <v>37878</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="D73">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B74">
-        <v>37806</v>
+        <v>40980</v>
       </c>
       <c r="C74">
         <v>0</v>
       </c>
       <c r="D74">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B75">
-        <v>37908</v>
+        <v>37824</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B76">
-        <v>37848</v>
+        <v>37968</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="D76">
-        <v>23</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B77">
-        <v>37608</v>
+        <v>37852</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -3584,13 +3584,13 @@
         <v>144</v>
       </c>
       <c r="B78">
-        <v>37910</v>
+        <v>37956</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -3598,21 +3598,21 @@
         <v>142</v>
       </c>
       <c r="B79">
-        <v>37946</v>
+        <v>37836</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B80">
-        <v>37944</v>
+        <v>37822</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -3623,10 +3623,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B81">
-        <v>37934</v>
+        <v>37954</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -3640,41 +3640,41 @@
         <v>144</v>
       </c>
       <c r="B82">
-        <v>37786</v>
+        <v>40872</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B83">
-        <v>37812</v>
+        <v>40950</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B84">
-        <v>37994</v>
+        <v>37900</v>
       </c>
       <c r="C84">
         <v>0</v>
       </c>
       <c r="D84">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -3682,21 +3682,21 @@
         <v>154</v>
       </c>
       <c r="B85">
-        <v>37842</v>
+        <v>40874</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="D85">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B86">
-        <v>40900</v>
+        <v>37822</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -3707,16 +3707,16 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B87">
-        <v>37950</v>
+        <v>37918</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
       <c r="D87">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -3724,7 +3724,7 @@
         <v>146</v>
       </c>
       <c r="B88">
-        <v>37852</v>
+        <v>37786</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -3735,10 +3735,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B89">
-        <v>37832</v>
+        <v>40824</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -3749,24 +3749,24 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B90">
-        <v>37866</v>
+        <v>37954</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B91">
-        <v>37882</v>
+        <v>37920</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -3777,27 +3777,27 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B92">
-        <v>37940</v>
+        <v>37794</v>
       </c>
       <c r="C92">
         <v>0</v>
       </c>
       <c r="D92">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>240</v>
+        <v>144</v>
       </c>
       <c r="B93">
-        <v>37920</v>
+        <v>37950</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93">
         <v>23</v>
@@ -3808,7 +3808,7 @@
         <v>142</v>
       </c>
       <c r="B94">
-        <v>37874</v>
+        <v>40936</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -3819,38 +3819,38 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B95">
-        <v>37872</v>
+        <v>37784</v>
       </c>
       <c r="C95">
         <v>0</v>
       </c>
       <c r="D95">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B96">
-        <v>37908</v>
+        <v>52770</v>
       </c>
       <c r="C96">
         <v>0</v>
       </c>
       <c r="D96">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B97">
-        <v>37932</v>
+        <v>68178</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3861,24 +3861,24 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="B98">
-        <v>37848</v>
+        <v>40956</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B99">
-        <v>37852</v>
+        <v>37810</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -3889,45 +3889,45 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>240</v>
+        <v>154</v>
       </c>
       <c r="B100">
-        <v>37818</v>
+        <v>37820</v>
       </c>
       <c r="C100">
         <v>0</v>
       </c>
       <c r="D100">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B101">
-        <v>105318</v>
+        <v>37864</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B103">
-        <f>AVERAGE(B2:B101)</f>
-        <v>38840.33</v>
+        <f>AVERAGE(B2:B101)-AVERAGE(A2:A101)</f>
+        <v>40316.120000000003</v>
       </c>
       <c r="D103">
-        <f>AVERAGE(D2:D101)</f>
-        <v>23.88</v>
+        <f>AVERAGE(D2:D101)-AVERAGE(C2:C101)</f>
+        <v>25.84</v>
       </c>
     </row>
   </sheetData>
@@ -3941,7 +3941,7 @@
   <sheetViews>
     <sheetView showRuler="0" zoomScale="135" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="H103" sqref="H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3958,28 +3958,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -6884,7 +6884,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H102" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -6903,7 +6903,7 @@
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -6921,28 +6921,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -9847,7 +9847,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H102" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -9866,7 +9866,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9877,213 +9877,213 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1">
         <f>VALUE(Loops!B103)</f>
-        <v>38840.33</v>
+        <v>40316.120000000003</v>
       </c>
       <c r="C2" s="1">
         <f>VALUE(Loops!D103)</f>
-        <v>23.88</v>
+        <v>25.84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1">
         <f>VALUE('Reading Time'!B103)</f>
-        <v>164886.87</v>
+        <v>34745.43</v>
       </c>
       <c r="C3" s="1">
         <f>VALUE('Reading Time'!D103)</f>
-        <v>98.01</v>
+        <v>21.65</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1">
         <f>VALUE('Procedure cycles'!B103)</f>
-        <v>196.53</v>
+        <v>13.069999999999993</v>
       </c>
       <c r="C4" s="1">
         <f>VALUE('Procedure time'!B103)</f>
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1">
         <f>VALUE('Procedure cycles'!C103)</f>
-        <v>197.52</v>
+        <v>14.060000000000002</v>
       </c>
       <c r="C5" s="1">
         <f>VALUE('Procedure time'!C103)</f>
-        <v>0.15</v>
+        <v>6.9999999999999993E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1">
         <f>VALUE('Procedure cycles'!D103)</f>
-        <v>244.44</v>
+        <v>427.9</v>
       </c>
       <c r="C6" s="1">
         <f>VALUE('Procedure time'!D103)</f>
-        <v>0.14000000000000001</v>
+        <v>6.0000000000000012E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1">
         <f>VALUE('Procedure cycles'!E103)</f>
-        <v>227.5</v>
+        <v>44.039999999999992</v>
       </c>
       <c r="C7" s="1">
         <f>VALUE('Procedure time'!E103)</f>
-        <v>0.15</v>
+        <v>6.9999999999999993E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1">
         <f>VALUE('Procedure cycles'!F103)</f>
-        <v>214.1</v>
+        <v>30.639999999999986</v>
       </c>
       <c r="C8" s="1">
         <f>VALUE('Procedure time'!F103)</f>
-        <v>0.12</v>
+        <v>3.9999999999999994E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1">
         <f>VALUE('Procedure cycles'!G103)</f>
-        <v>234.51</v>
+        <v>51.049999999999983</v>
       </c>
       <c r="C9" s="1">
         <f>VALUE('Procedure time'!G103)</f>
-        <v>0.3</v>
+        <v>0.21999999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1">
         <f>VALUE('Procedure cycles'!H103)</f>
-        <v>250.5</v>
+        <v>67.039999999999992</v>
       </c>
       <c r="C10" s="1">
         <f>VALUE('Procedure time'!H103)</f>
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1">
         <f>VALUE('Procedure cycles'!I103)</f>
-        <v>221.95</v>
+        <v>405.40999999999997</v>
       </c>
       <c r="C11" s="1">
         <f>VALUE('Procedure time'!I103)</f>
-        <v>0.14000000000000001</v>
+        <v>6.0000000000000012E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1">
         <f>VALUE('System Call'!B103)</f>
-        <v>4847.25</v>
+        <v>4682.63</v>
       </c>
       <c r="C12" s="1">
         <f>VALUE('System Call'!D103)</f>
-        <v>2.1</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1">
         <f>VALUE('Process creation'!B103)</f>
-        <v>486234.8</v>
+        <v>486080.99</v>
       </c>
       <c r="C13" s="1">
         <f>VALUE('Process creation'!D103)</f>
-        <v>153.46</v>
+        <v>153.41</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1">
         <f>VALUE('Process running'!B103)</f>
-        <v>1863987.92</v>
+        <v>750607.35999999987</v>
       </c>
       <c r="C14" s="1">
         <f>VALUE('Process running'!D103)</f>
-        <v>1314.86</v>
+        <v>522.40999999999985</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1">
         <f>VALUE('Thread creation'!B103)</f>
-        <v>35167.360000000001</v>
+        <v>35012.160000000003</v>
       </c>
       <c r="C15" s="1">
         <f>VALUE('Thread creation'!D103)</f>
-        <v>21.39</v>
+        <v>21.34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1">
         <f>VALUE('Thread running'!B103)</f>
-        <v>39940.1</v>
+        <v>39771.93</v>
       </c>
       <c r="C16" s="1">
         <f>VALUE('Thread running'!D103)</f>
-        <v>25.58</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1">
         <f>VALUE('Context switch cycles'!H103)</f>
@@ -10105,16 +10105,16 @@
   <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C110" sqref="C110"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -10122,1428 +10122,1428 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>332</v>
+        <v>51075</v>
       </c>
       <c r="B2">
-        <v>315344</v>
+        <v>95085</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D2">
-        <v>88</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>268</v>
+        <v>37926</v>
       </c>
       <c r="B3">
-        <v>261836</v>
+        <v>72470</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D3">
-        <v>86</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>198</v>
+        <v>37864</v>
       </c>
       <c r="B4">
-        <v>261420</v>
+        <v>70340</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D4">
-        <v>111</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>174</v>
+        <v>37804</v>
       </c>
       <c r="B5">
-        <v>139752</v>
+        <v>70642</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D5">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>354</v>
+        <v>37822</v>
       </c>
       <c r="B6">
-        <v>139978</v>
+        <v>72538</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>102</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>152</v>
+        <v>37848</v>
       </c>
       <c r="B7">
-        <v>144280</v>
+        <v>71838</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D7">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>284</v>
+        <v>37836</v>
       </c>
       <c r="B8">
-        <v>144950</v>
+        <v>71834</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D8">
-        <v>87</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>180</v>
+        <v>37852</v>
       </c>
       <c r="B9">
-        <v>140988</v>
+        <v>71382</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D9">
-        <v>99</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>154</v>
+        <v>37860</v>
       </c>
       <c r="B10">
-        <v>138800</v>
+        <v>69902</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D10">
-        <v>90</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>166</v>
+        <v>37876</v>
       </c>
       <c r="B11">
-        <v>151338</v>
+        <v>72094</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D11">
-        <v>94</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>168</v>
+        <v>37968</v>
       </c>
       <c r="B12">
-        <v>149956</v>
+        <v>72422</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D12">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>154</v>
+        <v>37794</v>
       </c>
       <c r="B13">
-        <v>141428</v>
+        <v>71484</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D13">
-        <v>89</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>144</v>
+        <v>37920</v>
       </c>
       <c r="B14">
-        <v>137650</v>
+        <v>71718</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D14">
-        <v>86</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>142</v>
+        <v>37854</v>
       </c>
       <c r="B15">
-        <v>139930</v>
+        <v>104792</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D15">
-        <v>87</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>152</v>
+        <v>40816</v>
       </c>
       <c r="B16">
-        <v>139758</v>
+        <v>70534</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D16">
-        <v>102</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>146</v>
+        <v>37822</v>
       </c>
       <c r="B17">
-        <v>140916</v>
+        <v>72510</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D17">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>154</v>
+        <v>37912</v>
       </c>
       <c r="B18">
-        <v>137242</v>
+        <v>71214</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D18">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>142</v>
+        <v>40890</v>
       </c>
       <c r="B19">
-        <v>141582</v>
+        <v>70620</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D19">
-        <v>88</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>144</v>
+        <v>37900</v>
       </c>
       <c r="B20">
-        <v>139632</v>
+        <v>71884</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D20">
-        <v>110</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>158</v>
+        <v>37822</v>
       </c>
       <c r="B21">
-        <v>152486</v>
+        <v>72762</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D21">
-        <v>87</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>168</v>
+        <v>37948</v>
       </c>
       <c r="B22">
-        <v>175516</v>
+        <v>74106</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D22">
-        <v>140</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>144</v>
+        <v>37956</v>
       </c>
       <c r="B23">
-        <v>140866</v>
+        <v>71568</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D23">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>144</v>
+        <v>37822</v>
       </c>
       <c r="B24">
-        <v>143826</v>
+        <v>69946</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D24">
-        <v>87</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>154</v>
+        <v>37912</v>
       </c>
       <c r="B25">
-        <v>146618</v>
+        <v>71996</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D25">
-        <v>115</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>166</v>
+        <v>37786</v>
       </c>
       <c r="B26">
-        <v>141802</v>
+        <v>72376</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D26">
-        <v>98</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>142</v>
+        <v>37820</v>
       </c>
       <c r="B27">
-        <v>187456</v>
+        <v>88957</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D27">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>154</v>
+        <v>37910</v>
       </c>
       <c r="B28">
-        <v>273784</v>
+        <v>70968</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D28">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>146</v>
+        <v>37850</v>
       </c>
       <c r="B29">
-        <v>157654</v>
+        <v>70368</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D29">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>152</v>
+        <v>37822</v>
       </c>
       <c r="B30">
-        <v>157094</v>
+        <v>70816</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D30">
-        <v>88</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>150</v>
+        <v>37980</v>
       </c>
       <c r="B31">
-        <v>158716</v>
+        <v>72702</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D31">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>152</v>
+        <v>37832</v>
       </c>
       <c r="B32">
-        <v>188562</v>
+        <v>85254</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D32">
-        <v>107</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>150</v>
+        <v>37832</v>
       </c>
       <c r="B33">
-        <v>152590</v>
+        <v>71080</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D33">
-        <v>94</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>252</v>
+        <v>37950</v>
       </c>
       <c r="B34">
-        <v>152732</v>
+        <v>106872</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D34">
-        <v>93</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>152</v>
+        <v>40978</v>
       </c>
       <c r="B35">
-        <v>155698</v>
+        <v>71670</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D35">
-        <v>97</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>176</v>
+        <v>37820</v>
       </c>
       <c r="B36">
-        <v>143850</v>
+        <v>73792</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D36">
-        <v>103</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>222</v>
+        <v>37908</v>
       </c>
       <c r="B37">
-        <v>248266</v>
+        <v>85616</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D37">
-        <v>98</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>142</v>
+        <v>37824</v>
       </c>
       <c r="B38">
-        <v>367722</v>
+        <v>72482</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D38">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>154</v>
+        <v>40898</v>
       </c>
       <c r="B39">
-        <v>148892</v>
+        <v>86006</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D39">
-        <v>96</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>144</v>
+        <v>37866</v>
       </c>
       <c r="B40">
-        <v>148918</v>
+        <v>71720</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D40">
-        <v>95</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>144</v>
+        <v>41012</v>
       </c>
       <c r="B41">
-        <v>292514</v>
+        <v>71020</v>
       </c>
       <c r="C41">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D41">
-        <v>103</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>144</v>
+        <v>37854</v>
       </c>
       <c r="B42">
-        <v>143060</v>
+        <v>69908</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D42">
-        <v>173</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>154</v>
+        <v>37822</v>
       </c>
       <c r="B43">
-        <v>169136</v>
+        <v>77194</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D43">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>156</v>
+        <v>37856</v>
       </c>
       <c r="B44">
-        <v>140820</v>
+        <v>72406</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D44">
-        <v>95</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>144</v>
+        <v>37918</v>
       </c>
       <c r="B45">
-        <v>156602</v>
+        <v>71744</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D45">
-        <v>91</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>144</v>
+        <v>37892</v>
       </c>
       <c r="B46">
-        <v>142154</v>
+        <v>71340</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D46">
-        <v>87</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>154</v>
+        <v>37928</v>
       </c>
       <c r="B47">
-        <v>144304</v>
+        <v>70924</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D47">
-        <v>85</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>154</v>
+        <v>37954</v>
       </c>
       <c r="B48">
-        <v>142578</v>
+        <v>71864</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D48">
-        <v>95</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>146</v>
+        <v>37822</v>
       </c>
       <c r="B49">
-        <v>140868</v>
+        <v>71614</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D49">
-        <v>93</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>168</v>
+        <v>37794</v>
       </c>
       <c r="B50">
-        <v>141574</v>
+        <v>70802</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D50">
-        <v>109</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>152</v>
+        <v>37856</v>
       </c>
       <c r="B51">
-        <v>142540</v>
+        <v>71230</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D51">
-        <v>132</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>144</v>
+        <v>37854</v>
       </c>
       <c r="B52">
-        <v>143954</v>
+        <v>70614</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D52">
-        <v>97</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>290</v>
+        <v>37864</v>
       </c>
       <c r="B53">
-        <v>196834</v>
+        <v>73910</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D53">
-        <v>94</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>166</v>
+        <v>37832</v>
       </c>
       <c r="B54">
-        <v>145884</v>
+        <v>72548</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D54">
-        <v>103</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>142</v>
+        <v>37908</v>
       </c>
       <c r="B55">
-        <v>158086</v>
+        <v>71060</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D55">
-        <v>99</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>144</v>
+        <v>37860</v>
       </c>
       <c r="B56">
-        <v>147564</v>
+        <v>69686</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D56">
-        <v>116</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>144</v>
+        <v>37952</v>
       </c>
       <c r="B57">
-        <v>155246</v>
+        <v>73628</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D57">
-        <v>119</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>146</v>
+        <v>37832</v>
       </c>
       <c r="B58">
-        <v>142418</v>
+        <v>73040</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D58">
-        <v>88</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>144</v>
+        <v>37862</v>
       </c>
       <c r="B59">
-        <v>220268</v>
+        <v>72900</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D59">
-        <v>121</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>164</v>
+        <v>37836</v>
       </c>
       <c r="B60">
-        <v>175326</v>
+        <v>72328</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D60">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>154</v>
+        <v>37848</v>
       </c>
       <c r="B61">
-        <v>151548</v>
+        <v>70640</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D61">
-        <v>101</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>142</v>
+        <v>38002</v>
       </c>
       <c r="B62">
-        <v>268352</v>
+        <v>71970</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D62">
-        <v>103</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>154</v>
+        <v>37898</v>
       </c>
       <c r="B63">
-        <v>147342</v>
+        <v>71520</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D63">
-        <v>87</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>176</v>
+        <v>37954</v>
       </c>
       <c r="B64">
-        <v>183360</v>
+        <v>71988</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D64">
-        <v>148</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>144</v>
+        <v>37854</v>
       </c>
       <c r="B65">
-        <v>147758</v>
+        <v>71176</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D65">
-        <v>88</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>168</v>
+        <v>37952</v>
       </c>
       <c r="B66">
-        <v>222536</v>
+        <v>70764</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D66">
-        <v>87</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>142</v>
+        <v>37832</v>
       </c>
       <c r="B67">
-        <v>221952</v>
+        <v>72670</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D67">
-        <v>90</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>146</v>
+        <v>37856</v>
       </c>
       <c r="B68">
-        <v>161586</v>
+        <v>72200</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D68">
-        <v>96</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>154</v>
+        <v>37866</v>
       </c>
       <c r="B69">
-        <v>255422</v>
+        <v>71786</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D69">
-        <v>101</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>154</v>
+        <v>37812</v>
       </c>
       <c r="B70">
-        <v>152180</v>
+        <v>70634</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D70">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>144</v>
+        <v>37910</v>
       </c>
       <c r="B71">
-        <v>152138</v>
+        <v>99252</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D71">
-        <v>90</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>142</v>
+        <v>37784</v>
       </c>
       <c r="B72">
-        <v>145636</v>
+        <v>70782</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D72">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>154</v>
+        <v>37894</v>
       </c>
       <c r="B73">
-        <v>181884</v>
+        <v>72078</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D73">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>156</v>
+        <v>37954</v>
       </c>
       <c r="B74">
-        <v>137870</v>
+        <v>72146</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D74">
-        <v>123</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>142</v>
+        <v>37934</v>
       </c>
       <c r="B75">
-        <v>170932</v>
+        <v>71520</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D75">
-        <v>88</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>144</v>
+        <v>37938</v>
       </c>
       <c r="B76">
-        <v>152784</v>
+        <v>72928</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D76">
-        <v>90</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>144</v>
+        <v>37918</v>
       </c>
       <c r="B77">
-        <v>148302</v>
+        <v>71620</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D77">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>154</v>
+        <v>37860</v>
       </c>
       <c r="B78">
-        <v>139410</v>
+        <v>70780</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D78">
-        <v>90</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>152</v>
+        <v>37814</v>
       </c>
       <c r="B79">
-        <v>160702</v>
+        <v>70632</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D79">
-        <v>93</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>144</v>
+        <v>37954</v>
       </c>
       <c r="B80">
-        <v>183209</v>
+        <v>71544</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D80">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>152</v>
+        <v>37820</v>
       </c>
       <c r="B81">
-        <v>139930</v>
+        <v>72410</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D81">
-        <v>92</v>
+        <v>44</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>154</v>
+        <v>37822</v>
       </c>
       <c r="B82">
-        <v>172468</v>
+        <v>70490</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D82">
-        <v>106</v>
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>146</v>
+        <v>37852</v>
       </c>
       <c r="B83">
-        <v>169552</v>
+        <v>77914</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D83">
-        <v>125</v>
+        <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>152</v>
+        <v>37910</v>
       </c>
       <c r="B84">
-        <v>165324</v>
+        <v>77472</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D84">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>144</v>
+        <v>37964</v>
       </c>
       <c r="B85">
-        <v>154124</v>
+        <v>71778</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D85">
-        <v>89</v>
+        <v>46</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>152</v>
+        <v>37820</v>
       </c>
       <c r="B86">
-        <v>141150</v>
+        <v>73672</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D86">
-        <v>87</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>144</v>
+        <v>37784</v>
       </c>
       <c r="B87">
-        <v>140280</v>
+        <v>71562</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D87">
-        <v>83</v>
+        <v>44</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>142</v>
+        <v>133830</v>
       </c>
       <c r="B88">
-        <v>140468</v>
+        <v>70354</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D88">
-        <v>202</v>
+        <v>44</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>154</v>
+        <v>37922</v>
       </c>
       <c r="B89">
-        <v>140492</v>
+        <v>69742</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D89">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>166</v>
+        <v>37784</v>
       </c>
       <c r="B90">
-        <v>140982</v>
+        <v>71686</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D90">
-        <v>89</v>
+        <v>47</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>142</v>
+        <v>37910</v>
       </c>
       <c r="B91">
-        <v>140760</v>
+        <v>71584</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D91">
-        <v>87</v>
+        <v>44</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>224</v>
+        <v>37960</v>
       </c>
       <c r="B92">
-        <v>140642</v>
+        <v>71044</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D92">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>142</v>
+        <v>37854</v>
       </c>
       <c r="B93">
-        <v>149072</v>
+        <v>72950</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D93">
-        <v>104</v>
+        <v>45</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>352</v>
+        <v>40980</v>
       </c>
       <c r="B94">
-        <v>140298</v>
+        <v>71408</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D94">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>154</v>
+        <v>37956</v>
       </c>
       <c r="B95">
-        <v>141572</v>
+        <v>71646</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D95">
-        <v>93</v>
+        <v>44</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>154</v>
+        <v>37866</v>
       </c>
       <c r="B96">
-        <v>155670</v>
+        <v>69946</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D96">
-        <v>131</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>164</v>
+        <v>37822</v>
       </c>
       <c r="B97">
-        <v>138494</v>
+        <v>73346</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D97">
-        <v>88</v>
+        <v>44</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>142</v>
+        <v>37864</v>
       </c>
       <c r="B98">
-        <v>145150</v>
+        <v>71494</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D98">
-        <v>105</v>
+        <v>44</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>166</v>
+        <v>37864</v>
       </c>
       <c r="B99">
-        <v>141828</v>
+        <v>70168</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D99">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>232</v>
+        <v>40936</v>
       </c>
       <c r="B100">
-        <v>137648</v>
+        <v>104820</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D100">
-        <v>96</v>
+        <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>144</v>
+        <v>37920</v>
       </c>
       <c r="B101">
-        <v>176322</v>
+        <v>72264</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D101">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B103">
-        <f>AVERAGE(B2:B101)</f>
-        <v>164886.87</v>
+        <f>AVERAGE(B2:B101)-AVERAGE(A2:A101)</f>
+        <v>34745.43</v>
       </c>
       <c r="D103">
-        <f>AVERAGE(D2:D101)</f>
-        <v>98.01</v>
+        <f>AVERAGE(D2:D101)-AVERAGE(C2:C101)</f>
+        <v>21.65</v>
       </c>
     </row>
   </sheetData>
@@ -11556,8 +11556,8 @@
   <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="117" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A102" sqref="A102:I103"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11568,31 +11568,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -14497,41 +14497,41 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B103">
-        <f>AVERAGE(B2:B101)</f>
-        <v>196.53</v>
+        <f>AVERAGE(B2:B101)-AVERAGE(A2:A101)</f>
+        <v>13.069999999999993</v>
       </c>
       <c r="C103">
-        <f t="shared" ref="C103:I103" si="0">AVERAGE(C2:C101)</f>
-        <v>197.52</v>
+        <f>AVERAGE(C2:C101)-AVERAGE(A2:A101)</f>
+        <v>14.060000000000002</v>
       </c>
       <c r="D103">
-        <f t="shared" si="0"/>
-        <v>244.44</v>
+        <f>AVERAGE(D2:D101)--AVERAGE(A2:A101)</f>
+        <v>427.9</v>
       </c>
       <c r="E103">
-        <f t="shared" si="0"/>
-        <v>227.5</v>
+        <f>AVERAGE(E2:E101)-AVERAGE(A2:A101)</f>
+        <v>44.039999999999992</v>
       </c>
       <c r="F103">
-        <f t="shared" si="0"/>
-        <v>214.1</v>
+        <f>AVERAGE(F2:F101)-AVERAGE(A2:A101)</f>
+        <v>30.639999999999986</v>
       </c>
       <c r="G103">
-        <f t="shared" si="0"/>
-        <v>234.51</v>
+        <f>AVERAGE(G2:G101)-AVERAGE(A2:A101)</f>
+        <v>51.049999999999983</v>
       </c>
       <c r="H103">
-        <f t="shared" si="0"/>
-        <v>250.5</v>
+        <f>AVERAGE(H2:H101)-AVERAGE(A2:A101)</f>
+        <v>67.039999999999992</v>
       </c>
       <c r="I103">
-        <f t="shared" si="0"/>
-        <v>221.95</v>
+        <f>AVERAGE(I2:I101)--AVERAGE(A2:A101)</f>
+        <v>405.40999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -14545,7 +14545,7 @@
   <sheetViews>
     <sheetView showRuler="0" zoomScale="113" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
+      <selection pane="bottomLeft" activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14556,31 +14556,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -17485,41 +17485,41 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B103">
-        <f>AVERAGE(B2:B101)</f>
-        <v>0.16</v>
+        <f>AVERAGE(B2:B101)-AVERAGE(A2:A101)</f>
+        <v>0.08</v>
       </c>
       <c r="C103">
-        <f t="shared" ref="C103:I103" si="0">AVERAGE(C2:C101)</f>
-        <v>0.15</v>
+        <f>AVERAGE(C2:C101)-AVERAGE(A2:A101)</f>
+        <v>6.9999999999999993E-2</v>
       </c>
       <c r="D103">
-        <f t="shared" si="0"/>
-        <v>0.14000000000000001</v>
+        <f>AVERAGE(D2:D101)-AVERAGE(A2:A101)</f>
+        <v>6.0000000000000012E-2</v>
       </c>
       <c r="E103">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
+        <f>AVERAGE(E2:E101)-AVERAGE(A2:A101)</f>
+        <v>6.9999999999999993E-2</v>
       </c>
       <c r="F103">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
+        <f>AVERAGE(F2:F101)-AVERAGE(A2:A101)</f>
+        <v>3.9999999999999994E-2</v>
       </c>
       <c r="G103">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
+        <f>AVERAGE(G2:G101)-AVERAGE(A2:A101)</f>
+        <v>0.21999999999999997</v>
       </c>
       <c r="H103">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
+        <f>AVERAGE(H2:H101)-AVERAGE(A2:A101)</f>
+        <v>0.08</v>
       </c>
       <c r="I103">
-        <f t="shared" si="0"/>
-        <v>0.14000000000000001</v>
+        <f>AVERAGE(I2:I101)-AVERAGE(A2:A101)</f>
+        <v>6.0000000000000012E-2</v>
       </c>
     </row>
   </sheetData>
@@ -17533,7 +17533,7 @@
   <sheetViews>
     <sheetView showRuler="0" zoomScale="117" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C105" sqref="C105"/>
+      <selection pane="bottomLeft" activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17546,16 +17546,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -18960,17 +18960,17 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B103">
-        <f>AVERAGE(B2:B101)</f>
-        <v>4847.25</v>
+        <f>AVERAGE(B2:B101)-AVERAGE(A2:A101)</f>
+        <v>4682.63</v>
       </c>
       <c r="D103">
-        <f>AVERAGE(D2:D101)</f>
-        <v>2.1</v>
+        <f>AVERAGE(D2:D101)-AVERAGE(C2:C101)</f>
+        <v>2.06</v>
       </c>
     </row>
   </sheetData>
@@ -18984,7 +18984,7 @@
   <sheetViews>
     <sheetView showRuler="0" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
+      <selection pane="bottomLeft" activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18997,16 +18997,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -20411,7 +20411,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -20420,16 +20420,16 @@
         <v>153.81</v>
       </c>
       <c r="B103">
-        <f>AVERAGE(B2:B101)</f>
-        <v>486234.8</v>
+        <f>AVERAGE(B2:B101)-A103</f>
+        <v>486080.99</v>
       </c>
       <c r="C103">
         <f>AVERAGE(C2:C101)</f>
         <v>0.05</v>
       </c>
       <c r="D103">
-        <f>AVERAGE(D2:D101)</f>
-        <v>153.46</v>
+        <f>AVERAGE(D2:D101)-C103</f>
+        <v>153.41</v>
       </c>
     </row>
   </sheetData>
@@ -20443,7 +20443,7 @@
   <sheetViews>
     <sheetView showRuler="0" zoomScale="134" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20456,16 +20456,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -21870,7 +21870,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -21879,16 +21879,16 @@
         <v>1113380.56</v>
       </c>
       <c r="B103">
-        <f>AVERAGE(B2:B101)</f>
-        <v>1863987.92</v>
+        <f>AVERAGE(B2:B101)-A103</f>
+        <v>750607.35999999987</v>
       </c>
       <c r="C103">
         <f>AVERAGE(C2:C101)</f>
         <v>792.45</v>
       </c>
       <c r="D103">
-        <f>AVERAGE(D2:D101)</f>
-        <v>1314.86</v>
+        <f>AVERAGE(D2:D101)-C103</f>
+        <v>522.40999999999985</v>
       </c>
     </row>
   </sheetData>
@@ -21902,7 +21902,7 @@
   <sheetViews>
     <sheetView showRuler="0" zoomScale="134" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D102"/>
+      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21915,16 +21915,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -23329,7 +23329,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -23338,16 +23338,16 @@
         <v>155.19999999999999</v>
       </c>
       <c r="B103">
-        <f t="shared" ref="B103:D103" si="0">AVERAGE(B2:B101)</f>
-        <v>35167.360000000001</v>
+        <f>AVERAGE(B2:B101)-A103</f>
+        <v>35012.160000000003</v>
       </c>
       <c r="C103">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B103:D103" si="0">AVERAGE(C2:C101)</f>
         <v>0.05</v>
       </c>
       <c r="D103">
-        <f t="shared" si="0"/>
-        <v>21.39</v>
+        <f>AVERAGE(D2:D101)-C103</f>
+        <v>21.34</v>
       </c>
     </row>
   </sheetData>
@@ -23361,7 +23361,7 @@
   <sheetViews>
     <sheetView showRuler="0" zoomScale="136" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23374,16 +23374,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -24788,7 +24788,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -24797,16 +24797,16 @@
         <v>168.17</v>
       </c>
       <c r="B103">
-        <f t="shared" ref="B103:D103" si="0">AVERAGE(B2:B101)</f>
-        <v>39940.1</v>
+        <f>AVERAGE(B2:B101)-A103</f>
+        <v>39771.93</v>
       </c>
       <c r="C103">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B103:D103" si="0">AVERAGE(C2:C101)</f>
         <v>0.08</v>
       </c>
       <c r="D103">
-        <f t="shared" si="0"/>
-        <v>25.58</v>
+        <f>AVERAGE(D2:D101)-C103</f>
+        <v>25.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>